<commit_message>
Updated CSVLib paper with performance related section
</commit_message>
<xml_diff>
--- a/plugins/vdm2isa/pub/csv-lib/results.xlsx
+++ b/plugins/vdm2isa/pub/csv-lib/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aray8\My Drive (abuh0018@gmail.com)\NCL\PhD\SAFE-CSV Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aray8\Documents\NCL\VDM\VDM_Toolkit\plugins\vdm2isa\pub\csv-lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E030EFB6-DA6D-4A5C-B0DE-B1204D6EC131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52398A14-8878-4E54-9FD0-A17195F10196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{3DE9090A-EBFB-4F0A-851D-DB938B249374}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Count</t>
   </si>
@@ -137,7 +137,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Parser Comparison: Default</a:t>
+              <a:t>Default</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -1442,16 +1442,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>212724</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>519018</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>75454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>125941</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>432235</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177053</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1487,6 +1487,25 @@
     <tableColumn id="2" xr3:uid="{A2E1E2E0-5430-43E3-9E3A-E6ABD05463F8}" name="VDM CSV"/>
     <tableColumn id="3" xr3:uid="{88636701-9897-4405-8C76-0D9A2FC5F97D}" name="SAFE-CSV: Native"/>
     <tableColumn id="4" xr3:uid="{3F9623AA-83E6-4D6F-9111-EF250BE2DDCB}" name="SAFE-CSV: Univocity"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{530E6202-8F61-4A15-87B0-F802750C00CD}" name="Table13" displayName="Table13" ref="A14:D25" totalsRowCount="1">
+  <autoFilter ref="A14:D24" xr:uid="{530E6202-8F61-4A15-87B0-F802750C00CD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C3520FAE-D710-4515-892F-C141E5B0A2B9}" name="Count"/>
+    <tableColumn id="2" xr3:uid="{79D04F81-74C1-424E-922C-680705E0DCE1}" name="VDM CSV"/>
+    <tableColumn id="3" xr3:uid="{D8E7F920-A165-4E9F-9F37-0BDC4750BAB2}" name="SAFE-CSV: Native" totalsRowFunction="custom">
+      <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
+      <totalsRowFormula>AVERAGE(Table13[SAFE-CSV: Native])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{34711185-28AF-4832-AAE3-29F66024730E}" name="SAFE-CSV: Univocity" totalsRowFunction="custom">
+      <calculatedColumnFormula>B2/D2</calculatedColumnFormula>
+      <totalsRowFormula>AVERAGE(Table13[SAFE-CSV: Univocity])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1789,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6DE700-5C75-449B-B3CD-14D3A8718501}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1955,12 +1974,197 @@
         <v>122518</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="B15">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <f>B2/C2</f>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="D15">
+        <f>B2/D2</f>
+        <v>2.1111111111111112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>500</v>
+      </c>
+      <c r="B16">
+        <v>154</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C24" si="0">B3/C3</f>
+        <v>2.5245901639344264</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D24" si="1">B3/D3</f>
+        <v>1.4666666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1000</v>
+      </c>
+      <c r="B17">
+        <v>333</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1.85</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>1.1404109589041096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>5000</v>
+      </c>
+      <c r="B18">
+        <v>4351</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1.3635224067690379</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1.4936491589426708</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>10000</v>
+      </c>
+      <c r="B19">
+        <v>15538</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1.3076923076923077</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>1.4480894687791239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>15000</v>
+      </c>
+      <c r="B20">
+        <v>33716</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1.2505470865323987</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>1.4456116280066886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20000</v>
+      </c>
+      <c r="B21">
+        <v>62374</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>1.3255270316218972</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>1.5482797994340465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>25000</v>
+      </c>
+      <c r="B22">
+        <v>94435</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1.2956001591460988</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>1.4504807544619545</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>30000</v>
+      </c>
+      <c r="B23">
+        <v>135664</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>1.3142425357952454</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1.4843213199413554</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>35000</v>
+      </c>
+      <c r="B24">
+        <v>186057</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1.3099008018924381</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1.5186095104392825</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <f>AVERAGE(Table13[SAFE-CSV: Native])</f>
+        <v>1.6708289160050516</v>
+      </c>
+      <c r="D25">
+        <f>AVERAGE(Table13[SAFE-CSV: Univocity])</f>
+        <v>1.5107230376687011</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated CSVLib paper to resolve typos
</commit_message>
<xml_diff>
--- a/plugins/vdm2isa/pub/csv-lib/results.xlsx
+++ b/plugins/vdm2isa/pub/csv-lib/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aray8\Documents\NCL\VDM\VDM_Toolkit\plugins\vdm2isa\pub\csv-lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52398A14-8878-4E54-9FD0-A17195F10196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46314853-7245-4DC9-9318-692461B179FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{3DE9090A-EBFB-4F0A-851D-DB938B249374}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Count</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>SAFE-CSV: Univocity</t>
+  </si>
+  <si>
+    <t>Standard CSV Library</t>
+  </si>
+  <si>
+    <t>SAFE-CSV: Native Parser</t>
+  </si>
+  <si>
+    <t>SAFE-CSV: Univocity Parser</t>
   </si>
 </sst>
 </file>
@@ -137,11 +146,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Default</a:t>
+              <a:t>Standard</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> VDM CSV, SAFE-CSV: Native and SAFE-CSV: Univocity</a:t>
+              <a:t> CSV Library, SAFE-CSV: Native Parser and SAFE-CSV: Univocity Parser</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -191,7 +200,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>VDM CSV</c:v>
+                  <c:v>Standard CSV Library</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -314,7 +323,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SAFE-CSV: Native</c:v>
+                  <c:v>SAFE-CSV: Native Parser</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -437,7 +446,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SAFE-CSV: Univocity</c:v>
+                  <c:v>SAFE-CSV: Univocity Parser</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -588,7 +597,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -601,14 +610,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1200"/>
                   <a:t>CSV</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0"/>
                   <a:t> Row Count</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB"/>
+                <a:endParaRPr lang="en-GB" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -625,7 +634,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -710,7 +719,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -723,7 +732,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1200"/>
                   <a:t>Time (ms)</a:t>
                 </a:r>
               </a:p>
@@ -742,7 +751,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -822,7 +831,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1484,9 +1493,9 @@
   <autoFilter ref="A1:D11" xr:uid="{EBF00B2C-BC24-43E3-B210-7B7A78882DB3}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C36C7622-EBCB-4377-849E-EE20D7E229B5}" name="Count"/>
-    <tableColumn id="2" xr3:uid="{A2E1E2E0-5430-43E3-9E3A-E6ABD05463F8}" name="VDM CSV"/>
-    <tableColumn id="3" xr3:uid="{88636701-9897-4405-8C76-0D9A2FC5F97D}" name="SAFE-CSV: Native"/>
-    <tableColumn id="4" xr3:uid="{3F9623AA-83E6-4D6F-9111-EF250BE2DDCB}" name="SAFE-CSV: Univocity"/>
+    <tableColumn id="2" xr3:uid="{A2E1E2E0-5430-43E3-9E3A-E6ABD05463F8}" name="Standard CSV Library"/>
+    <tableColumn id="3" xr3:uid="{88636701-9897-4405-8C76-0D9A2FC5F97D}" name="SAFE-CSV: Native Parser"/>
+    <tableColumn id="4" xr3:uid="{3F9623AA-83E6-4D6F-9111-EF250BE2DDCB}" name="SAFE-CSV: Univocity Parser"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1810,8 +1819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6DE700-5C75-449B-B3CD-14D3A8718501}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="142" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1825,13 +1834,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>